<commit_message>
data updates and script commit
</commit_message>
<xml_diff>
--- a/PostData.xlsx
+++ b/PostData.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taasj\Documents\Med School Research\Diagnostic Knee Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VHAMOURYAND15\Desktop\R local\Knee_Research_MedSchool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D8987C-6EA8-468A-95BB-3A13B37DA2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E3B28E-6327-4BD0-85BD-367D9E10D9F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{38D6511F-F27D-4A64-8E43-AF3B232FBF2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{38D6511F-F27D-4A64-8E43-AF3B232FBF2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="70">
   <si>
     <t>Subject</t>
   </si>
@@ -229,22 +228,7 @@
     <t>ACL, LCL</t>
   </si>
   <si>
-    <t>MCL, ACL</t>
-  </si>
-  <si>
-    <t>LCL, ACL</t>
-  </si>
-  <si>
-    <t>PCL, MCL</t>
-  </si>
-  <si>
-    <t>PCL, LCL</t>
-  </si>
-  <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Stand Alone</t>
   </si>
   <si>
     <t>GainedNew</t>
@@ -618,23 +602,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDEE26F-99AE-4D08-AEF0-63C8CD61F7DE}">
-  <dimension ref="A1:BB21"/>
+  <dimension ref="A1:BG22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -797,8 +781,23 @@
       <c r="BB1" t="s">
         <v>53</v>
       </c>
+      <c r="BC1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -961,8 +960,23 @@
       <c r="BB2">
         <v>0</v>
       </c>
+      <c r="BC2">
+        <v>10</v>
+      </c>
+      <c r="BD2">
+        <v>10</v>
+      </c>
+      <c r="BE2">
+        <v>10</v>
+      </c>
+      <c r="BF2">
+        <v>10</v>
+      </c>
+      <c r="BG2">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -985,13 +999,13 @@
         <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
         <v>59</v>
@@ -1125,8 +1139,23 @@
       <c r="BB3">
         <v>0</v>
       </c>
+      <c r="BC3">
+        <v>10</v>
+      </c>
+      <c r="BD3">
+        <v>9</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>64</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>64</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1179,7 +1208,7 @@
         <v>57</v>
       </c>
       <c r="R4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="S4">
         <v>1</v>
@@ -1289,8 +1318,23 @@
       <c r="BB4">
         <v>0</v>
       </c>
+      <c r="BC4">
+        <v>10</v>
+      </c>
+      <c r="BD4">
+        <v>10</v>
+      </c>
+      <c r="BE4">
+        <v>10</v>
+      </c>
+      <c r="BF4">
+        <v>10</v>
+      </c>
+      <c r="BG4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1331,19 +1375,19 @@
         <v>57</v>
       </c>
       <c r="N5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P5" t="s">
         <v>57</v>
       </c>
       <c r="Q5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="R5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -1453,8 +1497,23 @@
       <c r="BB5">
         <v>1</v>
       </c>
+      <c r="BC5">
+        <v>10</v>
+      </c>
+      <c r="BD5">
+        <v>10</v>
+      </c>
+      <c r="BE5">
+        <v>8</v>
+      </c>
+      <c r="BF5">
+        <v>8</v>
+      </c>
+      <c r="BG5">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1486,13 +1545,13 @@
         <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="L6" t="s">
         <v>55</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="N6" t="s">
         <v>60</v>
@@ -1507,7 +1566,7 @@
         <v>56</v>
       </c>
       <c r="R6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -1617,8 +1676,23 @@
       <c r="BB6">
         <v>1</v>
       </c>
+      <c r="BC6">
+        <v>9</v>
+      </c>
+      <c r="BD6">
+        <v>7</v>
+      </c>
+      <c r="BE6">
+        <v>9</v>
+      </c>
+      <c r="BF6">
+        <v>9</v>
+      </c>
+      <c r="BG6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1650,7 +1724,7 @@
         <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="L7" t="s">
         <v>55</v>
@@ -1781,8 +1855,23 @@
       <c r="BB7">
         <v>1</v>
       </c>
+      <c r="BC7">
+        <v>10</v>
+      </c>
+      <c r="BD7">
+        <v>10</v>
+      </c>
+      <c r="BE7">
+        <v>10</v>
+      </c>
+      <c r="BF7">
+        <v>10</v>
+      </c>
+      <c r="BG7">
+        <v>10</v>
+      </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1945,8 +2034,23 @@
       <c r="BB8">
         <v>0</v>
       </c>
+      <c r="BC8">
+        <v>10</v>
+      </c>
+      <c r="BD8">
+        <v>10</v>
+      </c>
+      <c r="BE8">
+        <v>10</v>
+      </c>
+      <c r="BF8">
+        <v>10</v>
+      </c>
+      <c r="BG8">
+        <v>10</v>
+      </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1990,7 +2094,7 @@
         <v>60</v>
       </c>
       <c r="O9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="P9" t="s">
         <v>57</v>
@@ -2109,186 +2213,30 @@
       <c r="BB9">
         <v>1</v>
       </c>
+      <c r="BC9">
+        <v>9</v>
+      </c>
+      <c r="BD9">
+        <v>7</v>
+      </c>
+      <c r="BE9">
+        <v>8</v>
+      </c>
+      <c r="BF9">
+        <v>8</v>
+      </c>
+      <c r="BG9">
+        <v>7</v>
+      </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" t="s">
-        <v>74</v>
-      </c>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14">
-        <v>10</v>
-      </c>
-      <c r="E14">
-        <v>10</v>
-      </c>
-      <c r="F14">
-        <v>8</v>
-      </c>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>10</v>
-      </c>
-      <c r="C15">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>10</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>10</v>
-      </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
-      </c>
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>8</v>
-      </c>
-      <c r="F17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18">
-        <v>9</v>
-      </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="D18">
-        <v>9</v>
-      </c>
-      <c r="E18">
-        <v>9</v>
-      </c>
-      <c r="F18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
-      <c r="D19">
-        <v>10</v>
-      </c>
-      <c r="E19">
-        <v>10</v>
-      </c>
-      <c r="F19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>8</v>
-      </c>
-      <c r="B20">
-        <v>10</v>
-      </c>
-      <c r="C20">
-        <v>10</v>
-      </c>
-      <c r="D20">
-        <v>10</v>
-      </c>
-      <c r="E20">
-        <v>10</v>
-      </c>
-      <c r="F20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>9</v>
-      </c>
-      <c r="B21">
-        <v>9</v>
-      </c>
-      <c r="C21">
-        <v>7</v>
-      </c>
-      <c r="D21">
-        <v>8</v>
-      </c>
-      <c r="E21">
-        <v>8</v>
-      </c>
-      <c r="F21">
-        <v>7</v>
-      </c>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>